<commit_message>
commit sửa lại export của report store checking
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Store_Checked.xlsx
+++ b/DMS/Templates/Report_Store_Checked.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RangDong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7064B62-2958-4303-B668-7F441302C02A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>STT</t>
   </si>
@@ -93,55 +92,52 @@
     <t>{{ReportStoreCheckeds.OrganizationName}}</t>
   </si>
   <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.STT}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.Username}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.DisplayName}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.dayOfWeek}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.StoreCheckings.StoreCode}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.StoreCheckings.StoreName}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.DateString}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.StoreCheckings.StoreAddress}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.StoreCheckings.eCheckIn}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.StoreCheckings.eCheckOut}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.StoreCheckings.Duaration}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.StoreCheckings.DeviceName}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.StoreCheckings.ePlanned}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.StoreCheckings.ImageCounter}}</t>
-  </si>
-  <si>
-    <t>{{ReportStoreCheckeds.SaleEmployees.StoreCheckingGroupByDates.StoreCheckings.eSalesOrder}}</t>
+    <t>{{ReportStoreCheckeds.Username}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.DisplayName}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.Date}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.DayOfWeek}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.StoreCode}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.StoreName}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.StoreAddress}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.CheckIn}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.CheckOut}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.Duration}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.Device}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.Planned}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.Image}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.Order}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -236,35 +232,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -272,34 +244,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,34 +533,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="5.44140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="16" style="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="9" style="1" customWidth="1"/>
-    <col min="9" max="10" width="7.5546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="27.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.88671875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.44140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
@@ -616,26 +569,16 @@
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
     </row>
-    <row r="4" spans="1:20" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
@@ -653,185 +596,130 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="L5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="11" t="s">
+      <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11" t="s">
+      <c r="D7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="11" t="s">
+      <c r="E7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="12"/>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="K7" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="T7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="10"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="13" t="s">
+      <c r="C8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="13" t="s">
+      <c r="D8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="13" t="s">
+      <c r="E8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9" s="5" t="s">
+      <c r="I8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="15" t="s">
+      <c r="J8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="15" t="s">
+      <c r="K8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="P9" s="15" t="s">
+      <c r="L8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="M8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="R9" s="15" t="s">
+      <c r="N8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="S9" s="15" t="s">
+      <c r="O8" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="T9" s="15" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="A4:T4"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A8:T8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="G7:H7"/>
+  <mergeCells count="3">
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
bổ sung thêm dữ liệu cho report store checker
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Store_Checked.xlsx
+++ b/DMS/Templates/Report_Store_Checked.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RangDong\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>STT</t>
   </si>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>{{ReportStoreCheckeds.Order}}</t>
+  </si>
+  <si>
+    <t>Khoảng cách Check-in</t>
+  </si>
+  <si>
+    <t>Khoảng cách Check-out</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.CheckInDistance}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.CheckOutDistance}}</t>
   </si>
 </sst>
 </file>
@@ -247,13 +259,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,52 +564,56 @@
     <col min="8" max="8" width="27.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="24.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
-    <row r="4" spans="1:15" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:17" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -615,13 +631,15 @@
       <c r="J5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
@@ -653,71 +671,83 @@
         <v>7</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="N8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="O8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="P8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="Q8" s="6" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A4:Q4"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
   </mergeCells>

</xml_diff>

<commit_message>
thêm api hình ảnh
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Store_Checked.xlsx
+++ b/DMS/Templates/Report_Store_Checked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7EFE1A-BF8F-4115-836A-367A7F223528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B57486E-4148-4BE6-B1AC-76FB31413DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>{{End}}</t>
   </si>
   <si>
-    <t>{{ReportStoreCheckeds.OrganizationName}}</t>
-  </si>
-  <si>
     <t>{{ReportStoreCheckeds.Username}}</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>{{ReportStoreCheckeds.CheckOutDistance}}</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.SaleEmployees.STT}}</t>
   </si>
 </sst>
 </file>
@@ -272,17 +272,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,7 +567,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -593,43 +593,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="4" spans="1:17" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -689,10 +689,10 @@
         <v>7</v>
       </c>
       <c r="K7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>8</v>
@@ -712,55 +712,55 @@
     </row>
     <row r="8" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="Q8" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="Q8" s="11" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thêm trạng thái đóng mở cửa hàng
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Store_Checked.xlsx
+++ b/DMS/Templates/Report_Store_Checked.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4984AEF-D1A4-43F7-9189-14E103546780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB46B2A0-EECC-44B0-8C2D-34B8AED1E379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Số giờ VT</t>
   </si>
   <si>
-    <t>Thiết bị</t>
-  </si>
-  <si>
     <t>Chụp ảnh</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>{{ReportStoreCheckeds.SalesEmployees.Dates.Contents.Duration}}</t>
   </si>
   <si>
-    <t>{{ReportStoreCheckeds.SalesEmployees.Dates.Contents.Device}}</t>
-  </si>
-  <si>
     <t>{{ReportStoreCheckeds.SalesEmployees.Dates.Contents.Planned}}</t>
   </si>
   <si>
@@ -160,6 +154,12 @@
   </si>
   <si>
     <t>{{ReportStoreCheckeds.SalesEmployees.Dates.Contents.StoreCodeDraft}}</t>
+  </si>
+  <si>
+    <t>Đóng cửa</t>
+  </si>
+  <si>
+    <t>{{ReportStoreCheckeds.SalesEmployees.Dates.Contents.Closed}}</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +656,7 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -686,7 +686,7 @@
     </row>
     <row r="4" spans="1:24" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -724,16 +724,16 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="M5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -765,16 +765,16 @@
       </c>
       <c r="J7" s="17"/>
       <c r="K7" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>5</v>
@@ -786,30 +786,30 @@
         <v>7</v>
       </c>
       <c r="R7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="T7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="U7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="V7" s="4" t="s">
+      <c r="W7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="W7" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="X7" s="4" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -837,66 +837,66 @@
     </row>
     <row r="9" spans="1:24" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="N9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="X9" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="U9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="W9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="X9" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>